<commit_message>
Klassendiagramm Wohnhaus getAnzahlBewohner hinzugefuegt
</commit_message>
<xml_diff>
--- a/Entwurf/Gebaeude_Tabellen.xlsx
+++ b/Entwurf/Gebaeude_Tabellen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mk/Documents/Hobby/Programmieren/Plebus/Entwurf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07568781-6400-6F4B-8019-BDD1F05743A5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DCABC5-2C15-2340-A243-E6DEAAEEC515}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{910F8A34-8214-7549-8ED7-46A70A19866D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{910F8A34-8214-7549-8ED7-46A70A19866D}"/>
   </bookViews>
   <sheets>
     <sheet name="Holzfäller" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="82">
   <si>
     <t>Level</t>
   </si>
@@ -212,10 +212,70 @@
     <t>1 Fisch / 1 Brot</t>
   </si>
   <si>
-    <t>Veränderung pro Intervall</t>
-  </si>
-  <si>
     <t>1 / 0 / -1</t>
+  </si>
+  <si>
+    <t>Bevölkerungsveränderung pro Intervall</t>
+  </si>
+  <si>
+    <t>Eigenschaften</t>
+  </si>
+  <si>
+    <t>Ausprägungen</t>
+  </si>
+  <si>
+    <t>GebäudeTyp</t>
+  </si>
+  <si>
+    <t>Wohnhaus</t>
+  </si>
+  <si>
+    <t>Geld</t>
+  </si>
+  <si>
+    <t>Verbraucht</t>
+  </si>
+  <si>
+    <t>Fisch, Brot</t>
+  </si>
+  <si>
+    <t>Pausierbar</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>Aktiv beim Verbessern</t>
+  </si>
+  <si>
+    <t>Ja, mit altem Level</t>
+  </si>
+  <si>
+    <t>Produzierendes Gebäude</t>
+  </si>
+  <si>
+    <t>Holz</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Maximales Level</t>
+  </si>
+  <si>
+    <t>Aktiv beim verbessern</t>
+  </si>
+  <si>
+    <t>Breite</t>
+  </si>
+  <si>
+    <t>Höhe</t>
+  </si>
+  <si>
+    <t>Lagerhaus</t>
+  </si>
+  <si>
+    <t>Stein</t>
   </si>
 </sst>
 </file>
@@ -251,9 +311,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -568,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7FD657-8D2A-4442-B237-7A0043E45275}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,9 +644,11 @@
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,8 +664,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -616,8 +687,15 @@
       <c r="E2" s="1">
         <v>1.1574074074074073E-4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -633,8 +711,15 @@
       <c r="E3" s="1">
         <v>1.0416666666666667E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -650,8 +735,15 @@
       <c r="E4" s="1">
         <v>9.2592592592592602E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -667,8 +759,15 @@
       <c r="E5" s="1">
         <v>8.1018518518518503E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -684,8 +783,15 @@
       <c r="E6" s="1">
         <v>6.9444444444444499E-5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -701,8 +807,14 @@
       <c r="E7" s="1">
         <v>5.7870370370370366E-5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -718,8 +830,14 @@
       <c r="E8" s="1">
         <v>4.6296296296296199E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -736,7 +854,7 @@
         <v>3.47222222222221E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -753,7 +871,7 @@
         <v>2.3148148148148001E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -777,10 +895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6ABB35-EEE7-D24E-9E6D-D0DA40411A2C}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E11" sqref="A1:E11"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,9 +908,11 @@
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -808,8 +928,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -825,8 +951,14 @@
       <c r="E2" s="1">
         <v>1.1574074074074073E-4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -842,8 +974,14 @@
       <c r="E3" s="1">
         <v>1.0416666666666667E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -859,8 +997,14 @@
       <c r="E4" s="1">
         <v>9.2592592592592602E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -876,8 +1020,14 @@
       <c r="E5" s="1">
         <v>8.1018518518518503E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -893,8 +1043,14 @@
       <c r="E6" s="1">
         <v>6.9444444444444499E-5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -910,8 +1066,14 @@
       <c r="E7" s="1">
         <v>5.7870370370370366E-5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -927,8 +1089,14 @@
       <c r="E8" s="1">
         <v>4.6296296296296199E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -945,7 +1113,7 @@
         <v>3.47222222222221E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -962,7 +1130,7 @@
         <v>2.3148148148148001E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1407,7 +1575,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:D11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1590,9 +1758,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DA892C-EF12-7748-AE11-1E454F1935E3}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1602,10 +1772,12 @@
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1625,10 +1797,16 @@
         <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1648,10 +1826,16 @@
         <v>59</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1671,10 +1855,16 @@
         <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1694,10 +1884,16 @@
         <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1717,10 +1913,16 @@
         <v>59</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1740,10 +1942,16 @@
         <v>59</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1763,10 +1971,16 @@
         <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1786,10 +2000,10 @@
         <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1809,10 +2023,10 @@
         <v>59</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1832,10 +2046,10 @@
         <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1855,7 +2069,7 @@
         <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>